<commit_message>
Update shared data - 2025-08-07T02-38-15-011Z
</commit_message>
<xml_diff>
--- a/Customer Capital Work details.xlsx
+++ b/Customer Capital Work details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/venkatanathandwarakanathan/Desktop/CC-Dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB587A6-0364-0241-8FD1-CA2344037CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C821D915-9739-114F-8248-D3C97E422A0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="25720" windowHeight="12980" xr2:uid="{0A6F300E-DE9E-4F51-9C84-70C237940D4C}"/>
   </bookViews>
@@ -174,9 +174,6 @@
     <t>HR-Recuitment Automation</t>
   </si>
   <si>
-    <t xml:space="preserve">DataWare house </t>
-  </si>
-  <si>
     <t>Order reconciliation</t>
   </si>
   <si>
@@ -186,10 +183,13 @@
     <t>NA</t>
   </si>
   <si>
-    <t>Price Grab - Competetive Prioce scraping from Portals</t>
-  </si>
-  <si>
     <t xml:space="preserve">Shepardti </t>
+  </si>
+  <si>
+    <t>Price Grab - Competetive Price scraping from Portals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Warehouse </t>
   </si>
 </sst>
 </file>
@@ -623,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8563BA6-12A6-4529-B2F8-0C9B569F1FE6}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -659,7 +659,7 @@
         <v>21</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>3</v>
@@ -696,7 +696,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>31</v>
@@ -774,7 +774,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>32</v>
@@ -786,7 +786,7 @@
         <v>5</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>22</v>
@@ -812,7 +812,7 @@
         <v>5</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>7</v>
@@ -838,7 +838,7 @@
         <v>17</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="3" t="s">
@@ -862,7 +862,7 @@
         <v>8</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>20</v>
@@ -978,7 +978,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>25</v>
@@ -1040,7 +1040,7 @@
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G16" s="4"/>
       <c r="H16" s="3" t="s">

</xml_diff>

<commit_message>
Update shared data - 2025-08-07T02-40-31-325Z
</commit_message>
<xml_diff>
--- a/Customer Capital Work details.xlsx
+++ b/Customer Capital Work details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/venkatanathandwarakanathan/Desktop/CC-Dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C821D915-9739-114F-8248-D3C97E422A0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA4E6FD-4127-A54F-93CD-284BD1C5757D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="25720" windowHeight="12980" xr2:uid="{0A6F300E-DE9E-4F51-9C84-70C237940D4C}"/>
   </bookViews>
@@ -135,9 +135,6 @@
     <t>DWH</t>
   </si>
   <si>
-    <t>Ganesh</t>
-  </si>
-  <si>
     <t>Ajay / Kushal</t>
   </si>
   <si>
@@ -190,6 +187,9 @@
   </si>
   <si>
     <t xml:space="preserve">Data Warehouse </t>
+  </si>
+  <si>
+    <t>Ganesh / Nishant</t>
   </si>
 </sst>
 </file>
@@ -623,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8563BA6-12A6-4529-B2F8-0C9B569F1FE6}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -659,7 +659,7 @@
         <v>21</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>3</v>
@@ -670,22 +670,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="F2" s="11">
         <v>44774</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>6</v>
@@ -696,22 +696,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F3" s="11">
         <v>43313</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>30</v>
@@ -722,13 +722,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>5</v>
@@ -754,7 +754,7 @@
         <v>29</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>5</v>
@@ -774,7 +774,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>32</v>
@@ -786,7 +786,7 @@
         <v>5</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>22</v>
@@ -812,7 +812,7 @@
         <v>5</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>7</v>
@@ -838,7 +838,7 @@
         <v>17</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="3" t="s">
@@ -853,7 +853,7 @@
         <v>9</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>26</v>
@@ -862,7 +862,7 @@
         <v>8</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>20</v>
@@ -882,7 +882,7 @@
         <v>31</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>8</v>
@@ -891,7 +891,7 @@
         <v>45883</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>6</v>
@@ -932,7 +932,7 @@
         <v>25</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>18</v>
@@ -958,7 +958,7 @@
         <v>25</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>18</v>
@@ -970,7 +970,7 @@
         <v>15</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -978,13 +978,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>18</v>
@@ -1004,13 +1004,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>18</v>
@@ -1030,21 +1030,21 @@
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G16" s="4"/>
       <c r="H16" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>